<commit_message>
Support the filtering of pkg...
</commit_message>
<xml_diff>
--- a/责任田信息.xlsx
+++ b/责任田信息.xlsx
@@ -791,7 +791,7 @@
     <t>/core/tests/coretests/src/com/android/internal/os/</t>
   </si>
   <si>
-    <t>core/tests/coretests/src/android/service/notification/</t>
+    <t>/core/tests/coretests/src/android/service/notification/</t>
   </si>
   <si>
     <t>/core/java/com/android/internal/midi/</t>
@@ -1679,7 +1679,7 @@
     <t xml:space="preserve"> /core/java/android/app/InstantAppResolvelnfo.aidl</t>
   </si>
   <si>
-    <t xml:space="preserve"> /core/java/android/app/InstantAppResolverService,java</t>
+    <t>/core/java/android/app/InstantAppResolverService.java</t>
   </si>
   <si>
     <t>/core/java/android/app/IntentService.java</t>
@@ -2119,10 +2119,10 @@
     <t>/core/java/com/android/internal/app/ChooserMultiProfilePagerAdapter.java;/core/java/com/android/internal/app/ChooserStackedAppDialogFragment.java;/core/java/com/android/internal/app/ChooserUtil.java;/core/java/com/android/internal/app/ConfirmUserCreationActivity.java;/core/java/com/android/internal/app/DisableCarModeActivity.java;/core/java/com/android/internal/app/EventLogTags.logtags;/core/java/com/android/internal/app/HarmfulAppWarningActivity.java;/core/java/com/android/internal/app/HeavyWeightSwitcherActivity.java;/core/java/com/android/internal/app/IAppOpsActiveCallback.aidl;/core/java/com/android/internal/app/IAppOpsAsyncNotedCallback.aidl;/core/java/com/android/internal/app/IAppOpsCallback.aidl;/core/java/com/android/internal/app/IAppOpsNotedCallback.aidl;/core/java/com/android/internal/app/IAppOpsService.aidl;/core/java/com/android/internal/app/IAppOpsStartedCallback.aidl;/core/java/com/android/internal/app/IBatteryStats.aidl;/core/java/com/android/internal/app/IHotwordRecognitionStatusCallback.aidl;/core/java/com/android/internal/app/IMediaContainerService.aidl;/core/java/com/android/internal/app/IntentForwarderActivity.java;/core/java/com/android/internal/app/ISoundTriggerService.aidl</t>
   </si>
   <si>
-    <t>/core/java/com/android/internal/app/ISoundTriggerSession.aidl;/core/java/com/android/internal/app/IVoiceActionCheckCallback.aidl;/core/java/com/android/internal/app/IVoicelnteractionManagerService.aidl;/core/java/com/android/internal/app/IVoicelnteractionSessionListener.aidl;/core/java/com/android/internal/IVoicelnteractionSessionShowCallback.aidl;/core/java/com/android/internal/app/IVoicelnteractionSoundTriggerSession.aidl;/core/java/com/android/internal/app/IVoicelnteractor.aidl;/core/java/com/android/internal/app/IVoicelnteractorRequest.aidl;/core/java/com/android/internal/app/LocaleHelper.java;/core/java/com/android/internal/app/LocalePicker.java;/core/java/com/android/internal/app/LocalePickerWithRegion.java;/core/java/com/android/internal/app/LocaleStore.java;/core/java/com/android/internal/app/MediaRouteChooserDialog.java;</t>
-  </si>
-  <si>
-    <t>/core/java/com/android/internal/app/MediaRouteControllerDialogFragment.java;/core/java/com/android/internal/app/MediaRouteDialogPresenter.java;/core/java/com/android/internal/app/MessageSamplingConfig.java;/core/java/com/android/internal/app/MessageSamplingConfig.aidl;/core/java/com/android/internal/app/MicroAlertController.java;/core/java/com/android/internal/app/NavltemSelectedListener.java;/core/java/com/android/internal/app/NetItenSelectedListener.java;/core/java/com/android/internal/app/OWNERS;/core/java/com/android/internal/app/package.html;/core/java/com/android/internal/app/PlatLogoActivity.java;/core/java/com/android/internal/app/ProcessMap.java;</t>
+    <t>/core/java/com/android/internal/app/ISoundTriggerSession.aidl;/core/java/com/android/internal/app/IVoiceActionCheckCallback.aidl;/core/java/com/android/internal/app/IVoicelnteractionManagerService.aidl;/core/java/com/android/internal/app/IVoicelnteractionSessionListener.aidl;/core/java/com/android/internal/IVoicelnteractionSessionShowCallback.aidl;/core/java/com/android/internal/app/IVoicelnteractionSoundTriggerSession.aidl;/core/java/com/android/internal/app/IVoicelnteractor.aidl;/core/java/com/android/internal/app/IVoicelnteractorRequest.aidl;/core/java/com/android/internal/app/LocaleHelper.java;/core/java/com/android/internal/app/LocalePicker.java;/core/java/com/android/internal/app/LocalePickerWithRegion.java;/core/java/com/android/internal/app/LocaleStore.java;/core/java/com/android/internal/app/MediaRouteChooserDialog.java</t>
+  </si>
+  <si>
+    <t>/core/java/com/android/internal/app/MediaRouteControllerDialogFragment.java;/core/java/com/android/internal/app/MediaRouteDialogPresenter.java;/core/java/com/android/internal/app/MessageSamplingConfig.java;/core/java/com/android/internal/app/MessageSamplingConfig.aidl;/core/java/com/android/internal/app/MicroAlertController.java;/core/java/com/android/internal/app/NavltemSelectedListener.java;/core/java/com/android/internal/app/NetItenSelectedListener.java;/core/java/com/android/internal/app/OWNERS;/core/java/com/android/internal/app/package.html;/core/java/com/android/internal/app/PlatLogoActivity.java;/core/java/com/android/internal/app/ProcessMap.java</t>
   </si>
   <si>
     <t>/core/java/com/android/internal/app/ResolverListAdapter.java;/core/java/com/android/internal/app/ResolverListController.java;/core/java/com/android/internal/app/ResolverMultiProfilePagerAdapter.java;/core/java/com/android/internal/app/ResolverRankerServiceResolverComparator.java;/core/java/com/android/internal/app/ResolverViewPager.java;/core/java/com/android/internal/app/ShutdownActivity.java;/core/java/com/android/internal/app/SimplelconFactory.java;/core/java/com/android/internal/app/SuggestedLocaleAdapter.java;/core/java/com/android/internal/app/SuspendedAppActivity.java;/core/java/com/android/internal/app/SystemUserHomeActivity.java;/core/java/com/android/internal/app/TEST_MAPPING;/core/java/com/android/internal/app/ToolbarActionBar.java;/core/java/com/android/internal/app/UnlaunchableAppActivity.java;/core/java/com/android/internal/app/WindowDecorActionBar.java</t>
@@ -2292,7 +2292,7 @@
 MagnificationSpec.aidl;/core/java/android/view/MagnificationSpec.java;/core/java/android/view/Menu.java;/core/java/android/view/Menulnflater.java;/core/java/android/view/Menultem.java</t>
   </si>
   <si>
-    <t>/core/java/android/view/NativeVectorDrawableAnimator.java;/core/java/android/view/OrientationEventListener.java;/core/java/android/view/OrientationListener.java;/core/java/android/view/OWNERS;/core/java/android/view/package.html;/core/java/android/view/PrivacyIndicatorBounds.java;/core/java/android/view/RemotableViewMethod.java;/core/java/android/view/RenderNodeAnimator,java;/core/java/android/view/RoundScrollbarRenderer.java;/core/java/android/view/ScaleGestureDetector.java;/core/java/android/view/SearchEvent.java;/core/java/android/view/SoundEffectConstants.java;/core/java/android/view/SubMenu.java;/core/java/android/view/Surface.java;/core/java/android/view/SurfaceControlFpsListener.java;/core/java/android/view/SurfaceControlHdrLayerlnfoListener.java;/core/java/android/view/SurfaceControlViewHost.aidl;/core/java/android/view/SurfaceControlViewHost.java;/core/java/android/view/SurfaceHolder.java;/core/java/android/view/SurfaceView.java;/core/java/android/view/TEST_MAPPING;/core/java/android/view/TextureView.java;/core/java/android/view/TouchDelegate.java;/core/java/android/view/TunnelModeEnabledListener.java</t>
+    <t>/core/java/android/view/NativeVectorDrawableAnimator.java;/core/java/android/view/OrientationEventListener.java;/core/java/android/view/OrientationListener.java;/core/java/android/view/OWNERS;/core/java/android/view/package.html;/core/java/android/view/PrivacyIndicatorBounds.java;/core/java/android/view/RemotableViewMethod.java;/core/java/android/view/RenderNodeAnimator.java;/core/java/android/view/RoundScrollbarRenderer.java;/core/java/android/view/ScaleGestureDetector.java;/core/java/android/view/SearchEvent.java;/core/java/android/view/SoundEffectConstants.java;/core/java/android/view/SubMenu.java;/core/java/android/view/Surface.java;/core/java/android/view/SurfaceControlFpsListener.java;/core/java/android/view/SurfaceControlHdrLayerlnfoListener.java;/core/java/android/view/SurfaceControlViewHost.aidl;/core/java/android/view/SurfaceControlViewHost.java;/core/java/android/view/SurfaceHolder.java;/core/java/android/view/SurfaceView.java;/core/java/android/view/TEST_MAPPING;/core/java/android/view/TextureView.java;/core/java/android/view/TouchDelegate.java;/core/java/android/view/TunnelModeEnabledListener.java</t>
   </si>
   <si>
     <t>平行世界</t>
@@ -3330,8 +3330,8 @@
   <sheetPr/>
   <dimension ref="A1:D731"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A699" workbookViewId="0">
-      <selection activeCell="C714" sqref="C714"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>

</xml_diff>